<commit_message>
fix error input after clear text in textbox
</commit_message>
<xml_diff>
--- a/TC1/dataEngine/DataEngine.xlsx
+++ b/TC1/dataEngine/DataEngine.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="103">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -322,25 +322,22 @@
     <t>DFJ 825-002</t>
   </si>
   <si>
-    <t>no</t>
+    <t>addSOItem</t>
+  </si>
+  <si>
+    <t>TS_025</t>
+  </si>
+  <si>
+    <t>TS_026</t>
+  </si>
+  <si>
+    <t>TS_027</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>addSOItem</t>
-  </si>
-  <si>
-    <t>TS_025</t>
-  </si>
-  <si>
-    <t>TS_026</t>
-  </si>
-  <si>
-    <t>TS_027</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -477,7 +474,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -512,7 +509,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -724,7 +721,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +752,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
@@ -769,10 +766,10 @@
         <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -784,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1188,7 @@
         <v>96</v>
       </c>
       <c r="H20" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,9 +1207,6 @@
       <c r="F21" t="s">
         <v>17</v>
       </c>
-      <c r="H21" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1230,9 +1224,6 @@
       <c r="F22" t="s">
         <v>17</v>
       </c>
-      <c r="H22" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1250,9 +1241,6 @@
       <c r="F23" t="s">
         <v>17</v>
       </c>
-      <c r="H23" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1264,9 +1252,6 @@
       <c r="F24" t="s">
         <v>20</v>
       </c>
-      <c r="H24" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1287,16 +1272,13 @@
       <c r="G25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H25" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
@@ -1313,7 +1295,7 @@
         <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
@@ -1324,7 +1306,7 @@
         <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -1606,7 +1588,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug getlaststepcount 20/5
finish build Keyword Driven Framework
</commit_message>
<xml_diff>
--- a/TC1/dataEngine/DataEngine.xlsx
+++ b/TC1/dataEngine/DataEngine.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="103">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -337,7 +337,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +752,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
@@ -769,7 +769,7 @@
         <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +782,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1188,7 @@
         <v>96</v>
       </c>
       <c r="H20" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1207,6 +1207,9 @@
       <c r="F21" t="s">
         <v>17</v>
       </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1224,6 +1227,9 @@
       <c r="F22" t="s">
         <v>17</v>
       </c>
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1241,6 +1247,9 @@
       <c r="F23" t="s">
         <v>17</v>
       </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1252,6 +1261,9 @@
       <c r="F24" t="s">
         <v>20</v>
       </c>
+      <c r="H24" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1272,6 +1284,9 @@
       <c r="G25" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="H25" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1289,6 +1304,9 @@
       <c r="F26" t="s">
         <v>17</v>
       </c>
+      <c r="H26" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1300,6 +1318,9 @@
       <c r="F27" t="s">
         <v>20</v>
       </c>
+      <c r="H27" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1310,6 +1331,9 @@
       </c>
       <c r="F28" t="s">
         <v>19</v>
+      </c>
+      <c r="H28" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>